<commit_message>
add shiny interactive app
</commit_message>
<xml_diff>
--- a/sample_profile/Sample Specs.xlsx
+++ b/sample_profile/Sample Specs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanju\Desktop\Lung Imaging\LAPD_Analysis\sample_profile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanju\Desktop\LAPD_Analysis\sample_profile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CAACEC-E4FC-4296-BAE7-4E0CE8359B8A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16977AB-EBE9-442C-B60A-879A62A7F6DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D7256AA9-00ED-4A7F-9B95-2BD91D614F66}"/>
   </bookViews>
@@ -190,8 +190,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A9CF87-BF1B-4ACF-BA9D-771153123C0A}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +577,7 @@
       <c r="F2">
         <v>10</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>74300000</v>
       </c>
       <c r="H2">
@@ -611,7 +612,7 @@
       <c r="F3">
         <v>10</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>124000000</v>
       </c>
       <c r="H3">
@@ -646,7 +647,7 @@
       <c r="F4">
         <v>10</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>109000000</v>
       </c>
       <c r="H4">
@@ -681,7 +682,7 @@
       <c r="F5">
         <v>10</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>383000000</v>
       </c>
       <c r="H5">
@@ -716,7 +717,7 @@
       <c r="F6">
         <v>10</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>137000000</v>
       </c>
       <c r="H6">
@@ -751,7 +752,7 @@
       <c r="F7">
         <v>10</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>112000000</v>
       </c>
       <c r="H7">
@@ -786,7 +787,7 @@
       <c r="F8">
         <v>10</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H8">
@@ -821,7 +822,7 @@
       <c r="F9">
         <v>10</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H9">
@@ -856,7 +857,7 @@
       <c r="F10">
         <v>10</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H10">
@@ -891,7 +892,7 @@
       <c r="F11">
         <v>10</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H11">
@@ -926,7 +927,7 @@
       <c r="F12">
         <v>10</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>624000000</v>
       </c>
       <c r="H12">
@@ -961,7 +962,7 @@
       <c r="F13">
         <v>10</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>373000000</v>
       </c>
       <c r="H13">
@@ -996,7 +997,7 @@
       <c r="F14">
         <v>10</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>265000000</v>
       </c>
       <c r="H14">
@@ -1031,7 +1032,7 @@
       <c r="F15">
         <v>10</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H15">
@@ -1066,7 +1067,7 @@
       <c r="F16">
         <v>15</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H16">
@@ -1101,7 +1102,7 @@
       <c r="F17">
         <v>15</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H17">
@@ -1136,7 +1137,7 @@
       <c r="F18">
         <v>15</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H18">
@@ -1171,7 +1172,7 @@
       <c r="F19">
         <v>15</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H19">
@@ -1186,6 +1187,15 @@
       <c r="K19" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G22" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:K19" xr:uid="{5A51B8E3-A1BE-4EDC-9F9E-3F7284F842DD}"/>

</xml_diff>